<commit_message>
modify genome and clone in model to fit latest requirements and discussions
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29140" windowHeight="18340" tabRatio="736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29140" windowHeight="20380" tabRatio="736"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="172">
   <si>
     <t>geid</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>genome</t>
-  </si>
-  <si>
-    <t>Homo sapiens [GRCh37]</t>
   </si>
   <si>
     <t>Homo sapiens [GRCh38]</t>
@@ -912,10 +909,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="42" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="41" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="42" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1200,24 +1197,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1227,77 +1206,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -1357,6 +1266,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1366,7 +1293,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -1391,6 +1318,41 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1401,6 +1363,41 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -1432,8 +1429,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C13" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="23"/>
-    <tableColumn id="2" name="Column names" dataDxfId="18"/>
-    <tableColumn id="3" name="Description" dataDxfId="17"/>
+    <tableColumn id="2" name="Column names" dataDxfId="22"/>
+    <tableColumn id="3" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1442,9 +1439,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A14:C24" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Sheet name" dataDxfId="22"/>
-    <tableColumn id="2" name="Column names" dataDxfId="16"/>
-    <tableColumn id="3" name="Description" dataDxfId="15"/>
+    <tableColumn id="1" name="Sheet name" dataDxfId="20"/>
+    <tableColumn id="2" name="Column names" dataDxfId="19"/>
+    <tableColumn id="3" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1453,9 +1450,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A25:C33" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Sheet name" dataDxfId="21"/>
-    <tableColumn id="2" name="Column names" dataDxfId="14"/>
-    <tableColumn id="3" name="Description" dataDxfId="13"/>
+    <tableColumn id="1" name="Sheet name" dataDxfId="17"/>
+    <tableColumn id="2" name="Column names" dataDxfId="16"/>
+    <tableColumn id="3" name="Description" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1464,9 +1461,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A34:C39" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Sheet name" dataDxfId="20"/>
-    <tableColumn id="2" name="Column names" dataDxfId="12"/>
-    <tableColumn id="3" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" name="Sheet name" dataDxfId="14"/>
+    <tableColumn id="2" name="Column names" dataDxfId="13"/>
+    <tableColumn id="3" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1475,7 +1472,7 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A40:C58" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Sheet name" dataDxfId="19"/>
+    <tableColumn id="1" name="Sheet name" dataDxfId="11"/>
     <tableColumn id="2" name="Column names" dataDxfId="10"/>
     <tableColumn id="3" name="Description" dataDxfId="9"/>
   </tableColumns>
@@ -1853,36 +1850,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="A1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1890,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1898,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1906,7 +1903,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1914,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1922,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1930,7 +1927,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1938,7 +1935,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1946,7 +1943,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1954,26 +1951,26 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1981,7 +1978,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1989,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1997,7 +1994,7 @@
         <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2005,7 +2002,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2013,7 +2010,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2021,7 +2018,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2029,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2037,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2045,26 +2042,26 @@
         <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2072,7 +2069,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2080,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2088,7 +2085,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2096,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2104,7 +2101,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2112,7 +2109,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2120,26 +2117,26 @@
         <v>20</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C34" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2147,7 +2144,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2155,7 +2152,7 @@
         <v>22</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2163,7 +2160,7 @@
         <v>23</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2171,26 +2168,26 @@
         <v>24</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C40" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2198,7 +2195,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2206,7 +2203,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2214,7 +2211,7 @@
         <v>26</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2222,7 +2219,7 @@
         <v>27</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2230,7 +2227,7 @@
         <v>28</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2238,7 +2235,7 @@
         <v>29</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2246,7 +2243,7 @@
         <v>30</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2254,7 +2251,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2262,7 +2259,7 @@
         <v>31</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2270,7 +2267,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2278,7 +2275,7 @@
         <v>33</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2286,7 +2283,7 @@
         <v>34</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2294,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2302,7 +2299,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2310,7 +2307,7 @@
         <v>37</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2318,7 +2315,7 @@
         <v>38</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2326,31 +2323,31 @@
         <v>8</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C59" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="C61" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2358,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2366,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2374,7 +2371,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2382,7 +2379,7 @@
         <v>40</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2390,7 +2387,7 @@
         <v>41</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2398,7 +2395,7 @@
         <v>42</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2406,7 +2403,7 @@
         <v>21</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2414,7 +2411,7 @@
         <v>43</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2422,7 +2419,7 @@
         <v>44</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2430,73 +2427,73 @@
         <v>45</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="B72" s="6"/>
       <c r="C72" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="B73" s="6"/>
       <c r="C73" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="B74" s="6"/>
       <c r="C74" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="B75" s="6"/>
       <c r="C75" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" s="6"/>
       <c r="C76" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" s="6"/>
       <c r="C77" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="B78" s="6"/>
       <c r="C78" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C79" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="C81" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2504,7 +2501,7 @@
         <v>46</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2512,7 +2509,7 @@
         <v>47</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2520,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2528,26 +2525,26 @@
         <v>8</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C86" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2555,7 +2552,7 @@
         <v>46</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2563,7 +2560,7 @@
         <v>39</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2571,7 +2568,7 @@
         <v>48</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2579,7 +2576,7 @@
         <v>49</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2587,7 +2584,7 @@
         <v>50</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2595,7 +2592,7 @@
         <v>51</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2603,7 +2600,7 @@
         <v>52</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2664,7 +2661,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>40</v>
@@ -2687,25 +2684,25 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2713,65 +2710,62 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
         <v>54</v>
       </c>
       <c r="H3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="F5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="G6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="G7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="G8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2924,7 +2918,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$B$2:$B$4</xm:f>
+            <xm:f>Menus!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
fix submission sheet for GEP00005; add new cell line and modify primer column geid to be 32 characters insyead of 8
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -18,7 +18,7 @@
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId9"/>
     <sheet name="Menus" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="173">
   <si>
     <t>geid</t>
   </si>
@@ -716,6 +716,9 @@
       </rPr>
       <t>ExperimentLayout@geid</t>
     </r>
+  </si>
+  <si>
+    <t>HUES9</t>
   </si>
 </sst>
 </file>
@@ -2633,7 +2636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -2754,6 +2759,9 @@
       </c>
     </row>
     <row r="6" spans="1:9">
+      <c r="F6" t="s">
+        <v>172</v>
+      </c>
       <c r="G6" t="s">
         <v>67</v>
       </c>
@@ -3239,7 +3247,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$F$2:$F$5</xm:f>
+            <xm:f>Menus!$F$2:$F$6</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
load project data with a new submission sheet
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
-    <sheet name="Project" sheetId="1" r:id="rId2"/>
-    <sheet name="Target" sheetId="2" r:id="rId3"/>
-    <sheet name="Guide" sheetId="3" r:id="rId4"/>
-    <sheet name="GuideMismatches" sheetId="4" r:id="rId5"/>
-    <sheet name="AmpliconSelection" sheetId="5" r:id="rId6"/>
-    <sheet name="ExperimentLayout" sheetId="6" r:id="rId7"/>
-    <sheet name="Plate" sheetId="7" r:id="rId8"/>
-    <sheet name="SequencingLibrary" sheetId="8" r:id="rId9"/>
-    <sheet name="Menus" sheetId="9" r:id="rId10"/>
+    <sheet name="Target" sheetId="2" r:id="rId2"/>
+    <sheet name="Guide" sheetId="3" r:id="rId3"/>
+    <sheet name="GuideMismatches" sheetId="4" r:id="rId4"/>
+    <sheet name="AmpliconSelection" sheetId="5" r:id="rId5"/>
+    <sheet name="ExperimentLayout" sheetId="6" r:id="rId6"/>
+    <sheet name="Plate" sheetId="7" r:id="rId7"/>
+    <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
+    <sheet name="Menus" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="152">
   <si>
     <t>geid</t>
   </si>
@@ -39,30 +38,9 @@
     <t>name</t>
   </si>
   <si>
-    <t>scientist</t>
-  </si>
-  <si>
-    <t>affiliation</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>group_leader</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>project_type</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>project_geid</t>
-  </si>
-  <si>
     <t>gene_id</t>
   </si>
   <si>
@@ -192,9 +170,6 @@
     <t>sequencing_sample_name</t>
   </si>
   <si>
-    <t>knock-in</t>
-  </si>
-  <si>
     <t>knock-out</t>
   </si>
   <si>
@@ -273,9 +248,6 @@
     <t>A549</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -295,50 +267,6 @@
   </si>
   <si>
     <t>SequencingLibrary</t>
-  </si>
-  <si>
-    <t>Unique ID for the project, in the format GEP-5digits (e.g. GEP00001)</t>
-  </si>
-  <si>
-    <t>Project name (e.g. STAT3_KO)</t>
-  </si>
-  <si>
-    <t>Name of the scientist submitting the job (e.g. 'Mary', who asks to make a KO line in STAT3)</t>
-  </si>
-  <si>
-    <t>Affiliation of the scientist</t>
-  </si>
-  <si>
-    <t>Group the scientist belongs to</t>
-  </si>
-  <si>
-    <t>Group leader in charge of the scientist</t>
-  </si>
-  <si>
-    <t>Date the project is submitted to Genome Editing</t>
-  </si>
-  <si>
-    <t>Brief description of the goals of the project</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> corresponds to a purchase code. Therefore one scientist can have several projects in an interval of time, all costed independently. Filling all fields is required.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -385,9 +313,6 @@
     <t>Strand location of the Target in the assembly either "forward" or "reverse"</t>
   </si>
   <si>
-    <t>The type of projecteither "knock-in" or "knock-out"</t>
-  </si>
-  <si>
     <t>Brief description of the Target</t>
   </si>
   <si>
@@ -647,23 +572,7 @@
     <t>The sample name assigned at the time of submission, in the format experiment_layout_geid_well_position: this must be 'one sample name per well', as per requirement of the Sequencing bioinformatics pipeline</t>
   </si>
   <si>
-    <t>Documentation for submitting new project to the Genome Editing Core App @ http://bioinf-ge001.cri.camres.org:8080/</t>
-  </si>
-  <si>
     <t>Genome Editing Core - Submission Form</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This ID must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Project@geid</t>
-    </r>
   </si>
   <si>
     <r>
@@ -693,19 +602,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">This must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Project@geid</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">This ID must match </t>
     </r>
     <r>
@@ -719,6 +615,9 @@
   </si>
   <si>
     <t>HUES9</t>
+  </si>
+  <si>
+    <t>Documentation for submitting new project's data to the Genome Editing Core App @ http://bioinf-ge001.cri.camres.org:8080/</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +905,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="21">
     <dxf>
       <font>
         <b val="0"/>
@@ -1371,76 +1270,13 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C13" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Sheet name" dataDxfId="23"/>
-    <tableColumn id="2" name="Column names" dataDxfId="22"/>
-    <tableColumn id="3" name="Description" dataDxfId="21"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A14:C24" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:C12" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="20"/>
     <tableColumn id="2" name="Column names" dataDxfId="19"/>
@@ -1450,8 +1286,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A25:C33" totalsRowShown="0">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:C21" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="17"/>
     <tableColumn id="2" name="Column names" dataDxfId="16"/>
@@ -1461,8 +1297,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A34:C39" totalsRowShown="0">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A22:C27" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="14"/>
     <tableColumn id="2" name="Column names" dataDxfId="13"/>
@@ -1472,8 +1308,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A40:C58" totalsRowShown="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A28:C46" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="11"/>
     <tableColumn id="2" name="Column names" dataDxfId="10"/>
@@ -1483,8 +1319,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A59:C78" totalsRowShown="0">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A47:C65" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="8"/>
     <tableColumn id="2" name="Column names" dataDxfId="7"/>
@@ -1494,8 +1330,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A79:C85" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A66:C72" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="5"/>
     <tableColumn id="2" name="Column names" dataDxfId="4"/>
@@ -1505,8 +1341,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A86:C94" totalsRowShown="0">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A73:C81" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Sheet name" dataDxfId="2"/>
     <tableColumn id="2" name="Column names" dataDxfId="1"/>
@@ -1838,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1854,249 +1690,252 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" s="6" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="6" t="s">
-        <v>8</v>
+      <c r="A13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
-        <v>81</v>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="6" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" s="6" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="B22" s="6" t="s">
-        <v>13</v>
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="6" t="s">
-        <v>14</v>
+      <c r="A23" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>116</v>
+      <c r="B25" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4" t="s">
-        <v>82</v>
+      <c r="B26" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>168</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="B28" s="6" t="s">
-        <v>1</v>
+      <c r="A28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="B29" s="6" t="s">
-        <v>16</v>
+      <c r="A29" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2104,7 +1943,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2112,7 +1951,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2120,490 +1959,380 @@
         <v>20</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>116</v>
+      <c r="B34" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="4" t="s">
-        <v>83</v>
+      <c r="B35" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" s="6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>116</v>
+      <c r="B40" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="4" t="s">
-        <v>84</v>
+      <c r="B41" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="B47" s="6" t="s">
-        <v>29</v>
+      <c r="A47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="B48" s="6" t="s">
-        <v>30</v>
+      <c r="A48" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="B49" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
       <c r="C49" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
       <c r="B50" s="6" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
       <c r="B51" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
       <c r="B52" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
       <c r="B53" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
       <c r="B54" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="6"/>
+      <c r="C59" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" s="6"/>
+      <c r="C60" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="7" t="s">
+    <row r="61" spans="2:3">
+      <c r="B61" s="6"/>
+      <c r="C61" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="6"/>
+      <c r="C62" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="6"/>
+      <c r="C63" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" s="6"/>
+      <c r="C64" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="B57" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="B58" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="7" t="s">
+    <row r="65" spans="1:3">
+      <c r="B65" s="6"/>
+      <c r="C65" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="7" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="C61" s="7" t="s">
+    <row r="68" spans="1:3">
+      <c r="C68" s="7" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="B63" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="B65" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="B66" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="B67" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="B68" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="B69" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="B71" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="B72" s="6"/>
-      <c r="C72" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="B73" s="6"/>
-      <c r="C73" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="B74" s="6"/>
-      <c r="C74" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="B75" s="6"/>
-      <c r="C75" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="B76" s="6"/>
-      <c r="C76" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="B77" s="6"/>
-      <c r="C77" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="B78" s="6"/>
-      <c r="C78" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="C81" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="B82" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="B83" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="B84" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="B85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="B88" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="B89" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="B90" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="B91" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="B92" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="B93" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="B94" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2614,7 +2343,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="8">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -2622,167 +2351,7 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="17">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="F6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="G7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="I12" s="3"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2793,7 +2362,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2801,111 +2370,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="6" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Menus!A2:A3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2920,15 +2414,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$C$2:$C$3</xm:f>
+            <xm:f>Menus!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$B$2:$B$3</xm:f>
+            <xm:f>Menus!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2939,7 +2433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2957,25 +2451,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2993,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -3011,16 +2505,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3035,7 +2529,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$E$2:$E$3</xm:f>
+            <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -3048,7 +2542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
@@ -3082,55 +2576,55 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3145,19 +2639,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$D$2:$D$4</xm:f>
+            <xm:f>Menus!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$C$2:$C$3</xm:f>
+            <xm:f>Menus!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$E$2:$E$3</xm:f>
+            <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
@@ -3170,9 +2664,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3180,47 +2674,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3235,21 +2725,21 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$E$2:$E$3</xm:f>
+            <xm:f>Menus!$D$2:$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Menus!$F$2:$F$8</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$G$2:$G$8</xm:f>
+            <xm:f>Menus!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Menus!$F$2:$F$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3260,7 +2750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -3278,16 +2768,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3305,7 +2795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -3324,25 +2814,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3357,13 +2847,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$H$2:$H$4</xm:f>
+            <xm:f>Menus!$G$2:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$I$2</xm:f>
+            <xm:f>Menus!$H$2</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -3374,4 +2864,153 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="17">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="H12" s="3"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new cell lines
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -17,7 +17,7 @@
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
     <sheet name="Menus" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
   <si>
     <t>geid</t>
   </si>
@@ -618,6 +618,15 @@
   </si>
   <si>
     <t>Documentation for submitting new project's data to the Genome Editing Core App @ http://bioinf-ge001.cri.camres.org:8080/</t>
+  </si>
+  <si>
+    <t>ZRTamR</t>
+  </si>
+  <si>
+    <t>ZRTamS</t>
+  </si>
+  <si>
+    <t>HEK293T</t>
   </si>
 </sst>
 </file>
@@ -714,7 +723,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -758,6 +767,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -818,7 +829,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -860,6 +871,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -902,6 +914,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
@@ -2669,7 +2682,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2737,7 +2750,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$E$2:$E$6</xm:f>
+            <xm:f>Menus!$E$2:$E$9</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -2871,7 +2884,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2991,13 +3004,24 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="E7" t="s">
+        <v>152</v>
+      </c>
       <c r="F7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8">
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
       <c r="F8" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="E9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:8">

</xml_diff>

<commit_message>
add water to the list of dna source
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="156">
   <si>
     <t>geid</t>
   </si>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>HEK293T</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -2813,7 +2816,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2860,15 +2863,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$G$2:$G$4</xm:f>
+            <xm:f>Menus!$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$H$2</xm:f>
+            <xm:f>Menus!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2884,7 +2887,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2994,6 +2997,9 @@
       <c r="F5" t="s">
         <v>58</v>
       </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="E6" t="s">

</xml_diff>

<commit_message>
add code to check that gene id is an Ensembl one, otherwise raise an error
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29140" windowHeight="20380" tabRatio="736"/>
+    <workbookView xWindow="35880" yWindow="0" windowWidth="29140" windowHeight="20380" tabRatio="736"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>Start location of the Target in the assembly</t>
   </si>
   <si>
-    <t>Target ID in the assembly, e.g. 'NC_000017.10'</t>
-  </si>
-  <si>
     <t>End location of the Target in the assembly</t>
   </si>
   <si>
@@ -630,6 +627,9 @@
   </si>
   <si>
     <t>water</t>
+  </si>
+  <si>
+    <t>Ensembl Gene ID must starts with ENSG, e.g. 'ENSG00000168610'</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1693,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1706,24 +1706,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>80</v>
@@ -1758,7 +1758,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1782,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1790,7 +1790,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1798,15 +1798,15 @@
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>80</v>
@@ -1817,7 +1817,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1825,7 +1825,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1841,7 +1841,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1849,7 +1849,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1857,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1865,7 +1865,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1873,15 +1873,15 @@
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>80</v>
@@ -1892,7 +1892,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1900,7 +1900,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1908,7 +1908,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1916,7 +1916,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1924,15 +1924,15 @@
         <v>17</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>80</v>
@@ -1943,7 +1943,7 @@
         <v>75</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1951,7 +1951,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1959,7 +1959,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1967,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1975,7 +1975,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1983,7 +1983,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1991,7 +1991,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1999,7 +1999,7 @@
         <v>23</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2007,7 +2007,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>24</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2023,7 +2023,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2031,7 +2031,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2039,7 +2039,7 @@
         <v>27</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2047,7 +2047,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2055,7 +2055,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2063,7 +2063,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2071,7 +2071,7 @@
         <v>31</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2079,15 +2079,15 @@
         <v>2</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>80</v>
@@ -2098,12 +2098,12 @@
         <v>76</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="C49" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -2119,7 +2119,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -2127,7 +2127,7 @@
         <v>33</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="2:3">
@@ -2135,7 +2135,7 @@
         <v>34</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -2143,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="2:3">
@@ -2151,7 +2151,7 @@
         <v>14</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="2:3">
@@ -2159,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="2:3">
@@ -2167,7 +2167,7 @@
         <v>37</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="2:3">
@@ -2175,57 +2175,57 @@
         <v>38</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="6"/>
       <c r="C59" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="6"/>
       <c r="C60" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="6"/>
       <c r="C61" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="B62" s="6"/>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" s="6"/>
       <c r="C63" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="6"/>
       <c r="C64" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="6"/>
       <c r="C65" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>80</v>
@@ -2236,12 +2236,12 @@
         <v>77</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="C68" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2249,7 +2249,7 @@
         <v>39</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2257,7 +2257,7 @@
         <v>40</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2265,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2273,15 +2273,15 @@
         <v>2</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>80</v>
@@ -2292,7 +2292,7 @@
         <v>78</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2300,7 +2300,7 @@
         <v>39</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2308,7 +2308,7 @@
         <v>32</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2316,7 +2316,7 @@
         <v>41</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2324,7 +2324,7 @@
         <v>42</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2332,7 +2332,7 @@
         <v>43</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2340,7 +2340,7 @@
         <v>44</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -2348,7 +2348,7 @@
         <v>45</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2563,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2998,12 +2998,12 @@
         <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="E6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" t="s">
         <v>59</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="E7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F7" t="s">
         <v>60</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="E8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
         <v>61</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="E9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:8">

</xml_diff>

<commit_message>
merge SequencingLibrary and ExperimentLayout into Layout, merge SequencingLibraryContent, WellContent and Well into LayoutContent, remove VariantResult, update load_layout(), link Guide to Project, remove VariantLoader, make UniqueConstraint works using __table_args__, remove unused tables in project view, and make the targets and guides ones work, add more test and check IntegrityError with right message is raised.
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -1300,7 +1300,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1344,6 +1344,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1495,7 +1499,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1576,6 +1580,8 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1657,6 +1663,8 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
@@ -4776,7 +4784,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5920,7 +5928,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$D$2:$D$3</xm:f>

</xml_diff>

<commit_message>
merge Amplicon and AmpliconSelection, move all related sequencing columns to LayoutContent to allow empty well in plate, add/check mandatory columns, add new properties on Amplicon: name, coordinates, fprimer and rprimer derived from existing columns, add border to table in webapp, update datatables library to 1.10.20, add Amplicon and Layout tables in webapp.
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -1300,7 +1300,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1344,6 +1344,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1499,7 +1509,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1582,6 +1592,11 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1665,6 +1680,11 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>

</xml_diff>

<commit_message>
update project spreadsheet: add drop down menus to validate input data for certain columns, mostly in layout tab
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736"/>
   </bookViews>
   <sheets>
-    <sheet name="Documentation" sheetId="10" r:id="rId1"/>
+    <sheet name="Help" sheetId="10" r:id="rId1"/>
     <sheet name="Target" sheetId="2" r:id="rId2"/>
     <sheet name="Guide" sheetId="3" r:id="rId3"/>
     <sheet name="Amplicon" sheetId="5" r:id="rId4"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
   <si>
     <t>description</t>
   </si>
@@ -115,12 +115,6 @@
     <t>plate_barcode</t>
   </si>
   <si>
-    <t>dna_source</t>
-  </si>
-  <si>
-    <t>library_type</t>
-  </si>
-  <si>
     <t>sequencing_barcode</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>knock-out</t>
   </si>
   <si>
-    <t>genome</t>
-  </si>
-  <si>
     <t>Homo sapiens [GRCh38]</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>non-fixed cells</t>
   </si>
   <si>
-    <t>Fluidigm</t>
-  </si>
-  <si>
     <t>MCF7</t>
   </si>
   <si>
@@ -197,9 +185,6 @@
   </si>
   <si>
     <t>MESC</t>
-  </si>
-  <si>
-    <t>is_it</t>
   </si>
   <si>
     <t>A549</t>
@@ -347,12 +332,6 @@
   </si>
   <si>
     <t>Ensembl Gene ID must starts with ENSG, e.g. 'ENSG00000168610'</t>
-  </si>
-  <si>
-    <t>GenEditID - Submission Form</t>
-  </si>
-  <si>
-    <t>Documentation for submitting new project's data to the GenEditID Web App</t>
   </si>
   <si>
     <r>
@@ -1183,12 +1162,21 @@
   <si>
     <t>NB. Orange tabs, tables and columns need to be filled, green ones are optionals.</t>
   </si>
+  <si>
+    <t>is_true_or_false</t>
+  </si>
+  <si>
+    <t>GenEditID - Project Data and Layout Spreadsheet</t>
+  </si>
+  <si>
+    <t>Help to fill project's data and layout before uploading into the GenEditID Web App</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1252,12 +1240,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <name val="Arial"/>
     </font>
@@ -1268,7 +1250,20 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
+      <sz val="16"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
       <color theme="3"/>
       <name val="Cambria"/>
       <scheme val="major"/>
@@ -1300,7 +1295,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1344,6 +1339,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1482,34 +1489,34 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1597,6 +1604,12 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1685,10 +1698,169 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="114">
+  <dxfs count="123">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3592,6 +3764,197 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:C12" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tab name" dataDxfId="122"/>
+    <tableColumn id="2" name="Column names" dataDxfId="121"/>
+    <tableColumn id="3" name="Description" dataDxfId="120"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Column1" headerRowDxfId="85" dataDxfId="84"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="83" dataDxfId="82"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="81" dataDxfId="80"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+  <tableColumns count="7">
+    <tableColumn id="1" name="target_name" dataDxfId="77"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="76"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="75"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="74"/>
+    <tableColumn id="5" name="target_start" dataDxfId="73"/>
+    <tableColumn id="6" name="target_end" dataDxfId="72"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="71"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="70">
+  <tableColumns count="1">
+    <tableColumn id="1" name="target_description" dataDxfId="69"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+  <tableColumns count="3">
+    <tableColumn id="1" name="target_name" dataDxfId="66"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="65"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="64"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <tableColumns count="4">
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="61"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="60"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="59"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="58"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:M9" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+  <tableColumns count="13">
+    <tableColumn id="1" name="guide_name" dataDxfId="55"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="54"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="53"/>
+    <tableColumn id="4" name="guide_strand" dataDxfId="52"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="51"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="50"/>
+    <tableColumn id="7" name="chrom" dataDxfId="49"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="48"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="47"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="46"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="45"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="44"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="43"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="N1:O9" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <tableColumns count="2">
+    <tableColumn id="1" name="score" dataDxfId="40"/>
+    <tableColumn id="2" name="description" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:D97" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <tableColumns count="4">
+    <tableColumn id="1" name="layout_id" dataDxfId="36"/>
+    <tableColumn id="2" name="well_position" dataDxfId="35"/>
+    <tableColumn id="6" name="guide_name" dataDxfId="34"/>
+    <tableColumn id="13" name="sequencing_barcode" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="E1:N97" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <tableColumns count="10">
+    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="30"/>
+    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="29"/>
+    <tableColumn id="3" name="sequencing_library_type" dataDxfId="28"/>
+    <tableColumn id="4" name="sequencing_project_id" dataDxfId="27"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="26"/>
+    <tableColumn id="6" name="cell_pool" dataDxfId="25"/>
+    <tableColumn id="7" name="clone_name" dataDxfId="24"/>
+    <tableColumn id="8" name="content_type" dataDxfId="23"/>
+    <tableColumn id="9" name="is_control" dataDxfId="22"/>
+    <tableColumn id="10" name="replicate_group" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <tableColumns count="4">
+    <tableColumn id="1" name="layout_id" dataDxfId="18"/>
+    <tableColumn id="2" name="plate_name" dataDxfId="17"/>
+    <tableColumn id="5" name="plate_barcode" dataDxfId="16"/>
+    <tableColumn id="4" name="plate_description" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:C18" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tab name" dataDxfId="119"/>
+    <tableColumn id="2" name="Column names" dataDxfId="118"/>
+    <tableColumn id="3" name="Description" dataDxfId="117"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <tableColumns count="4">
+    <tableColumn id="1" name="guide_name" dataDxfId="12"/>
+    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="11"/>
+    <tableColumn id="3" name="number_of_mismatches" dataDxfId="10"/>
+    <tableColumn id="4" name="number_of_off_targets" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <tableColumns count="7">
+    <tableColumn id="1" name="target_genome" dataDxfId="8"/>
+    <tableColumn id="2" name="strand" dataDxfId="7"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="6"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="5"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="4"/>
+    <tableColumn id="6" name="content_type" dataDxfId="3"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A69:C74" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tab name" dataDxfId="116"/>
+    <tableColumn id="2" name="Column names" dataDxfId="115"/>
+    <tableColumn id="3" name="Description" dataDxfId="114"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C37" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Tab name" dataDxfId="113"/>
     <tableColumn id="2" name="Column names" dataDxfId="112"/>
@@ -3601,139 +3964,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="76" dataDxfId="75"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="74" dataDxfId="73"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="72" dataDxfId="71"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
-  <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="68"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="67"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="66"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="65"/>
-    <tableColumn id="5" name="target_start" dataDxfId="64"/>
-    <tableColumn id="6" name="target_end" dataDxfId="63"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="62"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="61">
-  <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="60"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="57"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="56"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="55"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="52"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="51"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="50"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="49"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:M9" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <tableColumns count="13">
-    <tableColumn id="1" name="guide_name" dataDxfId="46"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="45"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="44"/>
-    <tableColumn id="4" name="guide_strand" dataDxfId="43"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="42"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="41"/>
-    <tableColumn id="7" name="chrom" dataDxfId="40"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="39"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="38"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="37"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="36"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="35"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="N1:O9" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <tableColumns count="2">
-    <tableColumn id="1" name="score" dataDxfId="31"/>
-    <tableColumn id="2" name="description" dataDxfId="30"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:D97" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="27"/>
-    <tableColumn id="2" name="well_position" dataDxfId="26"/>
-    <tableColumn id="6" name="guide_name" dataDxfId="25"/>
-    <tableColumn id="13" name="sequencing_barcode" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="E1:N97" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <tableColumns count="10">
-    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="21"/>
-    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="20"/>
-    <tableColumn id="3" name="sequencing_library_type" dataDxfId="19"/>
-    <tableColumn id="4" name="sequencing_project_id" dataDxfId="18"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="17"/>
-    <tableColumn id="6" name="cell_pool" dataDxfId="16"/>
-    <tableColumn id="7" name="clone_name" dataDxfId="15"/>
-    <tableColumn id="8" name="content_type" dataDxfId="14"/>
-    <tableColumn id="9" name="is_control" dataDxfId="13"/>
-    <tableColumn id="10" name="replicate_group" dataDxfId="12"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="9"/>
-    <tableColumn id="2" name="plate_name" dataDxfId="8"/>
-    <tableColumn id="5" name="plate_barcode" dataDxfId="7"/>
-    <tableColumn id="4" name="plate_description" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:C18" totalsRowShown="0">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A40:C45" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Tab name" dataDxfId="110"/>
     <tableColumn id="2" name="Column names" dataDxfId="109"/>
@@ -3743,20 +3975,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <tableColumns count="4">
-    <tableColumn id="1" name="guide_name" dataDxfId="3"/>
-    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="2"/>
-    <tableColumn id="3" name="number_of_mismatches" dataDxfId="1"/>
-    <tableColumn id="4" name="number_of_off_targets" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A69:C74" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A63:C68" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Tab name" dataDxfId="107"/>
     <tableColumn id="2" name="Column names" dataDxfId="106"/>
@@ -3766,56 +3986,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C37" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="104"/>
-    <tableColumn id="2" name="Column names" dataDxfId="103"/>
-    <tableColumn id="3" name="Description" dataDxfId="102"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A40:C45" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="101"/>
-    <tableColumn id="2" name="Column names" dataDxfId="100"/>
-    <tableColumn id="3" name="Description" dataDxfId="99"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A63:C68" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="98"/>
-    <tableColumn id="2" name="Column names" dataDxfId="97"/>
-    <tableColumn id="3" name="Description" dataDxfId="96"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A46:C62" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="95" dataDxfId="94"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="93" dataDxfId="92"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="91" dataDxfId="90"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="104" dataDxfId="103"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="102" dataDxfId="101"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="100" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A38:C39" headerRowCount="0" totalsRowShown="0" dataDxfId="89" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A38:C39" headerRowCount="0" totalsRowShown="0" dataDxfId="98" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="88" dataDxfId="87" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="86" dataDxfId="85" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="84" dataDxfId="83" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="97" dataDxfId="96" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="95" dataDxfId="94" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3824,9 +4011,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Table49" displayName="Table49" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="82" dataDxfId="81"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="80" dataDxfId="79"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="78" dataDxfId="77"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="91" dataDxfId="90"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="89" dataDxfId="88"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="87" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4154,6 +4341,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -4162,609 +4352,609 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="114.1640625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="114.1640625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27">
-      <c r="A1" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+    <row r="1" spans="1:3" ht="32">
+      <c r="A1" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" ht="20">
+      <c r="A2" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" ht="18">
+      <c r="A3" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="7" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="7" customFormat="1" ht="18" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="9" customFormat="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30">
+      <c r="A41" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="9" customFormat="1">
+      <c r="A43" s="2"/>
+      <c r="B43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="7" t="s">
+    <row r="53" spans="1:3">
+      <c r="B53" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" s="4"/>
+      <c r="C54" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" s="4"/>
+      <c r="C55" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" s="4"/>
+      <c r="C56" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" s="4"/>
+      <c r="C57" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" s="4"/>
+      <c r="C58" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" s="4"/>
+      <c r="C59" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="C63" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" customHeight="1">
+      <c r="A64" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="B65" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" customHeight="1">
+      <c r="A70" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C11" s="7" t="s">
+    <row r="71" spans="1:3">
+      <c r="B71" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row r="74" spans="1:3">
+      <c r="B74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
-      <c r="A24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="B25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="B29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="B30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="B31" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="B32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="B35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="11" customFormat="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="B37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30">
-      <c r="A41" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="B42" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="11" customFormat="1">
-      <c r="A43" s="4"/>
-      <c r="B43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="B44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="B45" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="B46" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="B47" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="B48" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="B49" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="B50" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="B51" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="B52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="B54" s="6"/>
-      <c r="C54" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="6"/>
-      <c r="C55" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="6"/>
-      <c r="C56" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="B57" s="6"/>
-      <c r="C57" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="B58" s="6"/>
-      <c r="C58" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="6"/>
-      <c r="C59" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="6"/>
-      <c r="C60" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="B61" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" customHeight="1">
-      <c r="A64" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="B65" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="B66" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="B67" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="B68" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="30" customHeight="1">
-      <c r="A70" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="B71" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="B72" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="B73" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="B74" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4809,53 +4999,53 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>202</v>
+      <c r="B1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -4905,37 +5095,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>217</v>
+      <c r="D1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4970,87 +5160,87 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="31.83203125" style="5" customWidth="1"/>
-    <col min="16" max="18" width="14.83203125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" style="5" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="31.83203125" style="3" customWidth="1"/>
+    <col min="16" max="18" width="14.83203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5106,833 +5296,833 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="12" spans="1:14">
+      <c r="A12" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B15" s="5" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B17" s="5" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" s="5" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="5" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" s="5" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B23" s="5" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B24" s="5" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="5" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B28" s="5" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" s="5" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B31" s="5" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B32" s="5" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B33" s="5" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B34" s="5" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35" s="5" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" s="5" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B37" s="5" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B38" s="5" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="5" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="5" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" s="5" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="5" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="5" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B44" s="5" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B45" s="5" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" s="5" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B47" s="5" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B48" s="5" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B49" s="5" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B50" s="5" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B51" s="5" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B52" s="5" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B53" s="5" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B54" s="5" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="5" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B56" s="5" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B57" s="5" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B58" s="5" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B59" s="5" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B60" s="5" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B61" s="5" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B62" s="5" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B63" s="5" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B64" s="5" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B65" s="5" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B66" s="5" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B67" s="5" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B68" s="5" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B69" s="5" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B70" s="5" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B71" s="5" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B72" s="5" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B73" s="5" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" s="5" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B75" s="5" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B76" s="5" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B77" s="5" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B78" s="5" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B79" s="5" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80" s="5" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B81" s="5" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B82" s="5" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" s="5" t="s">
+    <row r="90" spans="1:2">
+      <c r="A90" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B84" s="5" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B85" s="5" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B86" s="5" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B87" s="5" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B88" s="5" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B89" s="5" t="s">
+    <row r="96" spans="1:2">
+      <c r="A96" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B90" s="5" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -5948,18 +6138,30 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$F$2:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Menus!$G$2:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Menus!$E$2:$E$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5983,24 +6185,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.83203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="20.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>249</v>
+      <c r="D1" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6041,78 +6243,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="15">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="15">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -6144,26 +6346,29 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="17">
+    <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>196</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -6172,7 +6377,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>21</v>
@@ -6181,122 +6386,119 @@
         <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="E7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="E8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="E6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="E9" t="s">
-        <v>94</v>
+      <c r="E9" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="H12" s="3"/>
+      <c r="H12" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
remove cell line reference data it is now free text for cell_line_name, remove CellLine class, remove quide_strand, update loader and tests accordingly, add constraint on experiment_type now it is only knock-in or knock-out
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736"/>
+    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="736"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="241">
   <si>
     <t>description</t>
   </si>
@@ -61,9 +61,6 @@
     <t>guide_location</t>
   </si>
   <si>
-    <t>guide_strand</t>
-  </si>
-  <si>
     <t>score</t>
   </si>
   <si>
@@ -175,19 +172,7 @@
     <t>non-fixed cells</t>
   </si>
   <si>
-    <t>MCF7</t>
-  </si>
-  <si>
-    <t>T47D</t>
-  </si>
-  <si>
     <t>Mus musculus [GRCm38]</t>
-  </si>
-  <si>
-    <t>MESC</t>
-  </si>
-  <si>
-    <t>A549</t>
   </si>
   <si>
     <t>Target</t>
@@ -258,9 +243,6 @@
     <t>Coordinate of the cut side of the guide</t>
   </si>
   <si>
-    <t>The DNA strand that contains the guide sequence, either forward or reverse</t>
-  </si>
-  <si>
     <t>Chromosome where the amplicon is located, as a numeric value, e.g. 17</t>
   </si>
   <si>
@@ -314,18 +296,6 @@
       </rPr>
       <t>Guide@name</t>
     </r>
-  </si>
-  <si>
-    <t>HUES9</t>
-  </si>
-  <si>
-    <t>ZRTamR</t>
-  </si>
-  <si>
-    <t>ZRTamS</t>
-  </si>
-  <si>
-    <t>HEK293T</t>
   </si>
   <si>
     <t>water</t>
@@ -1170,6 +1140,9 @@
   </si>
   <si>
     <t>Help to fill project's data and layout before uploading into the GenEditID Web App</t>
+  </si>
+  <si>
+    <t>knock-in</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1268,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1339,6 +1312,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1506,17 +1481,17 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="191">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1610,6 +1585,7 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1704,10 +1680,147 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="122">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1727,142 +1840,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2405,23 +2382,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -3762,12 +3722,60 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>170822</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51" descr="amplicon.pptx.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="14372" t="18488" r="13531" b="23692"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="1866900"/>
+          <a:ext cx="10330822" cy="5854700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="122"/>
-    <tableColumn id="2" name="Column names" dataDxfId="121"/>
-    <tableColumn id="3" name="Description" dataDxfId="120"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="121"/>
+    <tableColumn id="2" name="Column names" dataDxfId="120"/>
+    <tableColumn id="3" name="Description" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3776,68 +3784,67 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="85" dataDxfId="84"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="83" dataDxfId="82"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="81" dataDxfId="80"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="84" dataDxfId="83"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="82" dataDxfId="81"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="80" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="77"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="76"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="75"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="74"/>
-    <tableColumn id="5" name="target_start" dataDxfId="73"/>
-    <tableColumn id="6" name="target_end" dataDxfId="72"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="71"/>
+    <tableColumn id="1" name="target_name" dataDxfId="76"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="75"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="74"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="73"/>
+    <tableColumn id="5" name="target_start" dataDxfId="72"/>
+    <tableColumn id="6" name="target_end" dataDxfId="71"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="69">
   <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="69"/>
+    <tableColumn id="1" name="target_description" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="66"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="65"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="64"/>
+    <tableColumn id="1" name="target_name" dataDxfId="65"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="64"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="61"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="60"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="59"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="58"/>
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="60"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="59"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="58"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:M9" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <tableColumns count="13">
-    <tableColumn id="1" name="guide_name" dataDxfId="55"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="54"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="53"/>
-    <tableColumn id="4" name="guide_strand" dataDxfId="52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:L9" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+  <tableColumns count="12">
+    <tableColumn id="1" name="guide_name" dataDxfId="54"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="53"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="52"/>
     <tableColumn id="5" name="is_on_target" dataDxfId="51"/>
     <tableColumn id="6" name="dna_feature" dataDxfId="50"/>
     <tableColumn id="7" name="chrom" dataDxfId="49"/>
@@ -3853,7 +3860,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="N1:O9" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="M1:N9" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <tableColumns count="2">
     <tableColumn id="1" name="score" dataDxfId="40"/>
     <tableColumn id="2" name="description" dataDxfId="39"/>
@@ -3907,9 +3914,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:C18" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="119"/>
-    <tableColumn id="2" name="Column names" dataDxfId="118"/>
-    <tableColumn id="3" name="Description" dataDxfId="117"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="118"/>
+    <tableColumn id="2" name="Column names" dataDxfId="117"/>
+    <tableColumn id="3" name="Description" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3928,81 +3935,81 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_genome" dataDxfId="8"/>
-    <tableColumn id="2" name="strand" dataDxfId="7"/>
-    <tableColumn id="3" name="dna_feature" dataDxfId="6"/>
-    <tableColumn id="4" name="is_true_or_false" dataDxfId="5"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="4"/>
-    <tableColumn id="6" name="content_type" dataDxfId="3"/>
-    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="2"/>
+    <tableColumn id="1" name="target_genome" dataDxfId="6"/>
+    <tableColumn id="2" name="strand" dataDxfId="5"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="4"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="3"/>
+    <tableColumn id="5" name="experiment_type" dataDxfId="2"/>
+    <tableColumn id="6" name="content_type" dataDxfId="1"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A69:C74" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A68:C73" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="116"/>
-    <tableColumn id="2" name="Column names" dataDxfId="115"/>
-    <tableColumn id="3" name="Description" dataDxfId="114"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="115"/>
+    <tableColumn id="2" name="Column names" dataDxfId="114"/>
+    <tableColumn id="3" name="Description" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C37" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C36" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="113"/>
-    <tableColumn id="2" name="Column names" dataDxfId="112"/>
-    <tableColumn id="3" name="Description" dataDxfId="111"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="112"/>
+    <tableColumn id="2" name="Column names" dataDxfId="111"/>
+    <tableColumn id="3" name="Description" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A40:C45" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A39:C44" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="110"/>
-    <tableColumn id="2" name="Column names" dataDxfId="109"/>
-    <tableColumn id="3" name="Description" dataDxfId="108"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="109"/>
+    <tableColumn id="2" name="Column names" dataDxfId="108"/>
+    <tableColumn id="3" name="Description" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A63:C68" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A62:C67" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="107"/>
-    <tableColumn id="2" name="Column names" dataDxfId="106"/>
-    <tableColumn id="3" name="Description" dataDxfId="105"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="106"/>
+    <tableColumn id="2" name="Column names" dataDxfId="105"/>
+    <tableColumn id="3" name="Description" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A46:C62" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A45:C61" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="104" dataDxfId="103"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="102" dataDxfId="101"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="100" dataDxfId="99"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="103" dataDxfId="102"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="101" dataDxfId="100"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="99" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A38:C39" headerRowCount="0" totalsRowShown="0" dataDxfId="98" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="97" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="97" dataDxfId="96" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="95" dataDxfId="94" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="96" dataDxfId="95" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="94" dataDxfId="93" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="92" dataDxfId="91" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4011,9 +4018,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Table49" displayName="Table49" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="91" dataDxfId="90"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="89" dataDxfId="88"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="87" dataDxfId="86"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="90" dataDxfId="89"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="88" dataDxfId="87"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="86" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4344,10 +4351,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -4359,43 +4366,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="32">
-      <c r="A1" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="A1" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" ht="20">
-      <c r="A2" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3" ht="18">
-      <c r="A3" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="A3" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4403,84 +4410,84 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="4" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="4" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="4" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="4" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="4" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="11" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4488,7 +4495,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4496,7 +4503,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4504,58 +4511,58 @@
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="4" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4563,7 +4570,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4571,7 +4578,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4579,15 +4586,15 @@
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -4595,23 +4602,23 @@
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="4" t="s">
-        <v>13</v>
+        <v>211</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>220</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="4" t="s">
-        <v>221</v>
+        <v>13</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4619,7 +4626,7 @@
         <v>14</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4627,7 +4634,7 @@
         <v>15</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4635,326 +4642,318 @@
         <v>16</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="9" customFormat="1">
+      <c r="A35" s="2"/>
       <c r="B35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="9" customFormat="1">
-      <c r="A36" s="2"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15">
+      <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>74</v>
+        <v>10</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30">
-      <c r="A41" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>217</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="9" customFormat="1">
+      <c r="A42" s="2"/>
       <c r="B42" s="4" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="9" customFormat="1">
-      <c r="A43" s="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="B43" s="4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="4" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="4" t="s">
-        <v>193</v>
+        <v>28</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="4" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="B49" s="4" t="s">
-        <v>194</v>
+        <v>20</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="B50" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="B51" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="B52" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="B53" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>223</v>
+      <c r="B53" s="4"/>
+      <c r="C53" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="4"/>
       <c r="C54" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="4"/>
       <c r="C55" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="4"/>
       <c r="C56" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="B57" s="4"/>
       <c r="C57" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" s="4"/>
       <c r="C58" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="B59" s="4"/>
       <c r="C59" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="B60" s="4"/>
-      <c r="C60" s="6" t="s">
-        <v>84</v>
+      <c r="B60" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="B61" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="B62" s="4" t="s">
-        <v>24</v>
+      <c r="A62" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" customHeight="1">
-      <c r="A64" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>237</v>
+        <v>51</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" s="4" t="s">
-        <v>241</v>
+        <v>26</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" s="4" t="s">
-        <v>27</v>
+        <v>232</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="B68" s="4" t="s">
-        <v>242</v>
+      <c r="A68" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="30" customHeight="1">
-      <c r="A70" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="B71" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="B72" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="B73" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="B74" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -5016,25 +5015,25 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5116,16 +5115,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5152,7 +5151,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5163,24 +5162,23 @@
     <col min="1" max="1" width="13" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="31.83203125" style="3" customWidth="1"/>
-    <col min="16" max="18" width="14.83203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="31.83203125" style="3" customWidth="1"/>
+    <col min="15" max="17" width="14.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1">
+    <row r="1" spans="1:14" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -5191,16 +5189,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>14</v>
@@ -5218,16 +5216,13 @@
         <v>18</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -5240,7 +5235,6 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5249,9 +5243,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5260,19 +5255,19 @@
           <x14:formula1>
             <xm:f>Menus!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$B$2:$B$3</xm:f>
+            <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$D$2:$D$3</xm:f>
+            <xm:f>Menus!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5315,814 +5310,814 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -6138,7 +6133,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$D$2:$D$3</xm:f>
@@ -6156,12 +6151,6 @@
             <xm:f>Menus!$G$2:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Menus!$E$2:$E$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6193,16 +6182,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -6351,7 +6340,9 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -6359,7 +6350,7 @@
     <col min="2" max="2" width="10.83203125" style="3"/>
     <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -6368,125 +6359,105 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>240</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="C4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="E5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="E6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="F7" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="E7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="3" t="s">
+    <row r="8" spans="1:8">
+      <c r="F8" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="E8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="E9" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8">

</xml_diff>

<commit_message>
update amplicon_id to include target name, remove guide_name on layout tab in submission spreadsheet and update loader and test spreadsheets
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="240">
   <si>
     <t>description</t>
   </si>
@@ -782,9 +782,6 @@
       </rPr>
       <t>Guide@guide_name</t>
     </r>
-  </si>
-  <si>
-    <t>This corresponds to the name of the guide used to edit the cell clone and must match Guide@guide_name</t>
   </si>
   <si>
     <t>Name of the guide</t>
@@ -1684,7 +1681,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="121">
     <dxf>
       <font>
         <b val="0"/>
@@ -2212,23 +2209,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -3773,9 +3753,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="121"/>
-    <tableColumn id="2" name="Column names" dataDxfId="120"/>
-    <tableColumn id="3" name="Description" dataDxfId="119"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="120"/>
+    <tableColumn id="2" name="Column names" dataDxfId="119"/>
+    <tableColumn id="3" name="Description" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3784,97 +3764,96 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="84" dataDxfId="83"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="82" dataDxfId="81"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="80" dataDxfId="79"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="83" dataDxfId="82"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="81" dataDxfId="80"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="79" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="76"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="75"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="74"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="73"/>
-    <tableColumn id="5" name="target_start" dataDxfId="72"/>
-    <tableColumn id="6" name="target_end" dataDxfId="71"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="70"/>
+    <tableColumn id="1" name="target_name" dataDxfId="75"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="74"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="73"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="72"/>
+    <tableColumn id="5" name="target_start" dataDxfId="71"/>
+    <tableColumn id="6" name="target_end" dataDxfId="70"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="68">
   <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="68"/>
+    <tableColumn id="1" name="target_description" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="65"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="64"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="63"/>
+    <tableColumn id="1" name="target_name" dataDxfId="64"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="63"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="60"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="59"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="58"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="57"/>
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="59"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="58"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="57"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:L9" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:L9" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <tableColumns count="12">
-    <tableColumn id="1" name="guide_name" dataDxfId="54"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="53"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="52"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="51"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="50"/>
-    <tableColumn id="7" name="chrom" dataDxfId="49"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="48"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="47"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="46"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="45"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="44"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="43"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="53"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="52"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="51"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="50"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="49"/>
+    <tableColumn id="7" name="chrom" dataDxfId="48"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="47"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="46"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="45"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="44"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="43"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="M1:N9" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="M1:N9" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="2">
-    <tableColumn id="1" name="score" dataDxfId="40"/>
-    <tableColumn id="2" name="description" dataDxfId="39"/>
+    <tableColumn id="1" name="score" dataDxfId="39"/>
+    <tableColumn id="2" name="description" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:D97" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="36"/>
-    <tableColumn id="2" name="well_position" dataDxfId="35"/>
-    <tableColumn id="6" name="guide_name" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C97" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <tableColumns count="3">
+    <tableColumn id="1" name="layout_id" dataDxfId="35"/>
+    <tableColumn id="2" name="well_position" dataDxfId="34"/>
     <tableColumn id="13" name="sequencing_barcode" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3882,7 +3861,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="E1:N97" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M97" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="10">
     <tableColumn id="1" name="sequencing_sample_name" dataDxfId="30"/>
     <tableColumn id="2" name="sequencing_dna_source" dataDxfId="29"/>
@@ -3914,9 +3893,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:C18" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="118"/>
-    <tableColumn id="2" name="Column names" dataDxfId="117"/>
-    <tableColumn id="3" name="Description" dataDxfId="116"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="117"/>
+    <tableColumn id="2" name="Column names" dataDxfId="116"/>
+    <tableColumn id="3" name="Description" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3950,11 +3929,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A68:C73" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A67:C72" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="115"/>
-    <tableColumn id="2" name="Column names" dataDxfId="114"/>
-    <tableColumn id="3" name="Description" dataDxfId="113"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="114"/>
+    <tableColumn id="2" name="Column names" dataDxfId="113"/>
+    <tableColumn id="3" name="Description" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3963,53 +3942,53 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C36" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="112"/>
-    <tableColumn id="2" name="Column names" dataDxfId="111"/>
-    <tableColumn id="3" name="Description" dataDxfId="110"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="111"/>
+    <tableColumn id="2" name="Column names" dataDxfId="110"/>
+    <tableColumn id="3" name="Description" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A39:C44" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A39:C43" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="109"/>
-    <tableColumn id="2" name="Column names" dataDxfId="108"/>
-    <tableColumn id="3" name="Description" dataDxfId="107"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="108"/>
+    <tableColumn id="2" name="Column names" dataDxfId="107"/>
+    <tableColumn id="3" name="Description" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A62:C67" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A61:C66" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="106"/>
-    <tableColumn id="2" name="Column names" dataDxfId="105"/>
-    <tableColumn id="3" name="Description" dataDxfId="104"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="105"/>
+    <tableColumn id="2" name="Column names" dataDxfId="104"/>
+    <tableColumn id="3" name="Description" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A45:C61" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A44:C60" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="103" dataDxfId="102"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="101" dataDxfId="100"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="99" dataDxfId="98"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="102" dataDxfId="101"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="100" dataDxfId="99"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="98" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="97" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="96" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="96" dataDxfId="95" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="94" dataDxfId="93" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="92" dataDxfId="91" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="95" dataDxfId="94" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="91" dataDxfId="90" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4018,9 +3997,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Table49" displayName="Table49" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="90" dataDxfId="89"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="88" dataDxfId="87"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="86" dataDxfId="85"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="89" dataDxfId="88"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="87" dataDxfId="86"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="85" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4351,10 +4330,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -4367,21 +4346,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32">
       <c r="A1" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -4410,7 +4389,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4418,7 +4397,7 @@
         <v>186</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4495,7 +4474,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4503,7 +4482,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4602,12 +4581,12 @@
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>65</v>
@@ -4668,7 +4647,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
@@ -4677,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4693,18 +4672,18 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="9" customFormat="1">
@@ -4718,55 +4697,55 @@
     </row>
     <row r="43" spans="1:3">
       <c r="B43" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="4" t="s">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="4" t="s">
-        <v>183</v>
+        <v>28</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="4" t="s">
-        <v>28</v>
+        <v>184</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="4" t="s">
-        <v>184</v>
+        <v>20</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="B49" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>223</v>
@@ -4774,185 +4753,177 @@
     </row>
     <row r="50" spans="1:3">
       <c r="B50" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="B51" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="B52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>213</v>
+      <c r="B52" s="4"/>
+      <c r="C52" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" s="4"/>
       <c r="C53" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="4"/>
       <c r="C54" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="4"/>
       <c r="C55" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="4"/>
       <c r="C56" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="B57" s="4"/>
       <c r="C57" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" s="4"/>
       <c r="C58" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="B59" s="4"/>
-      <c r="C59" s="6" t="s">
-        <v>78</v>
+      <c r="B59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="B61" s="4" t="s">
-        <v>23</v>
+      <c r="A61" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" customHeight="1">
-      <c r="A63" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C62" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63" s="4" t="s">
         <v>227</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="4" t="s">
-        <v>231</v>
+        <v>26</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" s="4" t="s">
-        <v>26</v>
+        <v>231</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="B67" s="4" t="s">
-        <v>232</v>
+      <c r="A67" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="30" customHeight="1">
-      <c r="A69" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="B71" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="B72" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="B73" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -5195,7 +5166,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -5283,7 +5254,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:N97"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -5293,66 +5264,62 @@
   <cols>
     <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="3"/>
+    <col min="3" max="3" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1">
+    <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>183</v>
+        <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>181</v>
       </c>
@@ -5360,7 +5327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -5368,7 +5335,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>181</v>
       </c>
@@ -5376,7 +5343,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>181</v>
       </c>
@@ -5384,7 +5351,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>181</v>
       </c>
@@ -5392,7 +5359,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>181</v>
       </c>
@@ -5400,7 +5367,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>181</v>
       </c>
@@ -5408,7 +5375,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -5416,7 +5383,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
         <v>181</v>
       </c>
@@ -5424,7 +5391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
         <v>181</v>
       </c>
@@ -5432,7 +5399,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
         <v>181</v>
       </c>
@@ -5440,7 +5407,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
         <v>181</v>
       </c>
@@ -5448,7 +5415,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
         <v>181</v>
       </c>
@@ -5456,7 +5423,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
         <v>181</v>
       </c>
@@ -5464,7 +5431,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
         <v>181</v>
       </c>
@@ -6138,19 +6105,19 @@
           <x14:formula1>
             <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$F$2:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6182,16 +6149,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -6368,7 +6335,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
@@ -6417,7 +6384,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
add new tab for desire edited sequences, update loader to generate amplicount_sequences.csv when spreadsheet has data, update geneditid_run_amplicount tool to pick up automatically amplicount_sequences.csv when in project folder, update submission spreadsheets
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -14,7 +14,8 @@
     <sheet name="Layout" sheetId="6" r:id="rId5"/>
     <sheet name="Plate" sheetId="7" r:id="rId6"/>
     <sheet name="GuideMismatches" sheetId="4" r:id="rId7"/>
-    <sheet name="Menus" sheetId="9" r:id="rId8"/>
+    <sheet name="DesireEditedSequences" sheetId="11" r:id="rId8"/>
+    <sheet name="Menus" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="246">
   <si>
     <t>description</t>
   </si>
@@ -283,19 +284,6 @@
   </si>
   <si>
     <t>- empty-vector: A control with vector that harbours neither guide nor Cas9</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This ID must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Guide@name</t>
-    </r>
   </si>
   <si>
     <t>water</t>
@@ -1140,6 +1128,54 @@
   </si>
   <si>
     <t>knock-in</t>
+  </si>
+  <si>
+    <t>sequence_name</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>DesireEditedSequences</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This name must match </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Guide@name</t>
+    </r>
+  </si>
+  <si>
+    <t>The name of the sequence</t>
+  </si>
+  <si>
+    <t>The sequence</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>DesireEditedSequences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> is the list of sequence to count the reads against. If not provided, all sequences above a certain threshold will be considered for counting the reads.   </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1265,7 +1301,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1309,6 +1345,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1488,7 +1538,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="205">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1583,6 +1633,13 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1678,10 +1735,224 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="121">
+  <dxfs count="128">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3173,109 +3444,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -3753,9 +3921,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="120"/>
-    <tableColumn id="2" name="Column names" dataDxfId="119"/>
-    <tableColumn id="3" name="Description" dataDxfId="118"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="127"/>
+    <tableColumn id="2" name="Column names" dataDxfId="126"/>
+    <tableColumn id="3" name="Description" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3764,127 +3932,126 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="83" dataDxfId="82"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="81" dataDxfId="80"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="79" dataDxfId="78"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="97" dataDxfId="96"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="95" dataDxfId="94"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="93" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A73:C76" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Tab name" dataDxfId="2"/>
+    <tableColumn id="2" name="Column names" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="75"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="74"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="73"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="72"/>
-    <tableColumn id="5" name="target_start" dataDxfId="71"/>
-    <tableColumn id="6" name="target_end" dataDxfId="70"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="69"/>
+    <tableColumn id="1" name="target_name" dataDxfId="89"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="88"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="87"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="86"/>
+    <tableColumn id="5" name="target_start" dataDxfId="85"/>
+    <tableColumn id="6" name="target_end" dataDxfId="84"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="68">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" dataDxfId="82">
   <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="67"/>
+    <tableColumn id="1" name="target_description" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="64"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="63"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="62"/>
+    <tableColumn id="1" name="target_name" dataDxfId="78"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="77"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="59"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="58"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="57"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="56"/>
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="73"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="72"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="71"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:L9" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:L9" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <tableColumns count="12">
-    <tableColumn id="1" name="guide_name" dataDxfId="53"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="52"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="51"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="50"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="49"/>
-    <tableColumn id="7" name="chrom" dataDxfId="48"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="47"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="46"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="45"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="44"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="43"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="42"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="67"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="66"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="65"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="64"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="63"/>
+    <tableColumn id="7" name="chrom" dataDxfId="62"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="61"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="60"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="59"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="58"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="57"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="M1:N9" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="M1:N9" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <tableColumns count="2">
-    <tableColumn id="1" name="score" dataDxfId="39"/>
-    <tableColumn id="2" name="description" dataDxfId="38"/>
+    <tableColumn id="1" name="score" dataDxfId="53"/>
+    <tableColumn id="2" name="description" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C97" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C97" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <tableColumns count="3">
-    <tableColumn id="1" name="layout_id" dataDxfId="35"/>
-    <tableColumn id="2" name="well_position" dataDxfId="34"/>
-    <tableColumn id="13" name="sequencing_barcode" dataDxfId="33"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="49"/>
+    <tableColumn id="2" name="well_position" dataDxfId="48"/>
+    <tableColumn id="13" name="sequencing_barcode" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M97" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M97" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <tableColumns count="10">
-    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="30"/>
-    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="29"/>
-    <tableColumn id="3" name="sequencing_library_type" dataDxfId="28"/>
-    <tableColumn id="4" name="sequencing_project_id" dataDxfId="27"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="26"/>
-    <tableColumn id="6" name="cell_pool" dataDxfId="25"/>
-    <tableColumn id="7" name="clone_name" dataDxfId="24"/>
-    <tableColumn id="8" name="content_type" dataDxfId="23"/>
-    <tableColumn id="9" name="is_control" dataDxfId="22"/>
-    <tableColumn id="10" name="replicate_group" dataDxfId="21"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="18"/>
-    <tableColumn id="2" name="plate_name" dataDxfId="17"/>
-    <tableColumn id="5" name="plate_barcode" dataDxfId="16"/>
-    <tableColumn id="4" name="plate_description" dataDxfId="15"/>
+    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="44"/>
+    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="43"/>
+    <tableColumn id="3" name="sequencing_library_type" dataDxfId="42"/>
+    <tableColumn id="4" name="sequencing_project_id" dataDxfId="41"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="40"/>
+    <tableColumn id="6" name="cell_pool" dataDxfId="39"/>
+    <tableColumn id="7" name="clone_name" dataDxfId="38"/>
+    <tableColumn id="8" name="content_type" dataDxfId="37"/>
+    <tableColumn id="9" name="is_control" dataDxfId="36"/>
+    <tableColumn id="10" name="replicate_group" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3893,36 +4060,58 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A14:C18" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="117"/>
-    <tableColumn id="2" name="Column names" dataDxfId="116"/>
-    <tableColumn id="3" name="Description" dataDxfId="115"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="124"/>
+    <tableColumn id="2" name="Column names" dataDxfId="123"/>
+    <tableColumn id="3" name="Description" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_name" dataDxfId="12"/>
-    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="11"/>
-    <tableColumn id="3" name="number_of_mismatches" dataDxfId="10"/>
-    <tableColumn id="4" name="number_of_off_targets" dataDxfId="9"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="32"/>
+    <tableColumn id="2" name="plate_name" dataDxfId="31"/>
+    <tableColumn id="5" name="plate_barcode" dataDxfId="30"/>
+    <tableColumn id="4" name="plate_description" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D11" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <tableColumns count="4">
+    <tableColumn id="1" name="guide_name" dataDxfId="26"/>
+    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="25"/>
+    <tableColumn id="3" name="number_of_mismatches" dataDxfId="24"/>
+    <tableColumn id="4" name="number_of_off_targets" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:B9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="2">
+    <tableColumn id="1" name="sequence_name" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="sequence" dataDxfId="5" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_genome" dataDxfId="6"/>
-    <tableColumn id="2" name="strand" dataDxfId="5"/>
-    <tableColumn id="3" name="dna_feature" dataDxfId="4"/>
-    <tableColumn id="4" name="is_true_or_false" dataDxfId="3"/>
-    <tableColumn id="5" name="experiment_type" dataDxfId="2"/>
-    <tableColumn id="6" name="content_type" dataDxfId="1"/>
-    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="0"/>
+    <tableColumn id="1" name="target_genome" dataDxfId="20"/>
+    <tableColumn id="2" name="strand" dataDxfId="19"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="18"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="17"/>
+    <tableColumn id="5" name="experiment_type" dataDxfId="16"/>
+    <tableColumn id="6" name="content_type" dataDxfId="15"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3931,9 +4120,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A67:C72" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="114"/>
-    <tableColumn id="2" name="Column names" dataDxfId="113"/>
-    <tableColumn id="3" name="Description" dataDxfId="112"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="121"/>
+    <tableColumn id="2" name="Column names" dataDxfId="120"/>
+    <tableColumn id="3" name="Description" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3942,9 +4131,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A23:C36" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="111"/>
-    <tableColumn id="2" name="Column names" dataDxfId="110"/>
-    <tableColumn id="3" name="Description" dataDxfId="109"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="118"/>
+    <tableColumn id="2" name="Column names" dataDxfId="117"/>
+    <tableColumn id="3" name="Description" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3953,9 +4142,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A39:C43" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="108"/>
-    <tableColumn id="2" name="Column names" dataDxfId="107"/>
-    <tableColumn id="3" name="Description" dataDxfId="106"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="115"/>
+    <tableColumn id="2" name="Column names" dataDxfId="114"/>
+    <tableColumn id="3" name="Description" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3964,9 +4153,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A61:C66" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="105"/>
-    <tableColumn id="2" name="Column names" dataDxfId="104"/>
-    <tableColumn id="3" name="Description" dataDxfId="103"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="112"/>
+    <tableColumn id="2" name="Column names" dataDxfId="111"/>
+    <tableColumn id="3" name="Description" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3975,20 +4164,20 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A44:C60" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="102" dataDxfId="101"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="100" dataDxfId="99"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="98" dataDxfId="97"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="109" dataDxfId="108"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="107" dataDxfId="106"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="105" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="96" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="7" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="95" dataDxfId="94" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="93" dataDxfId="92" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="91" dataDxfId="90" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="13" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="9" dataDxfId="8" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3997,9 +4186,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Table49" displayName="Table49" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="89" dataDxfId="88"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="87" dataDxfId="86"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="85" dataDxfId="84"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="103" dataDxfId="102"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="101" dataDxfId="100"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="99" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4330,7 +4519,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
@@ -4346,28 +4535,28 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32">
       <c r="A1" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>58</v>
@@ -4381,7 +4570,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4389,28 +4578,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>53</v>
@@ -4418,7 +4607,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>54</v>
@@ -4426,7 +4615,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>55</v>
@@ -4434,7 +4623,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>56</v>
@@ -4443,15 +4632,15 @@
     <row r="13" spans="1:3" ht="15">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>58</v>
@@ -4466,7 +4655,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4474,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4482,7 +4671,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4495,39 +4684,39 @@
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>58</v>
@@ -4538,7 +4727,7 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>62</v>
@@ -4549,7 +4738,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4573,7 +4762,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -4581,12 +4770,12 @@
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>65</v>
@@ -4647,7 +4836,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
@@ -4656,12 +4845,12 @@
         <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>58</v>
@@ -4672,22 +4861,21 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="9" customFormat="1">
-      <c r="A42" s="2"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="B42" s="4" t="s">
         <v>19</v>
       </c>
@@ -4700,23 +4888,23 @@
         <v>27</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -4724,15 +4912,15 @@
         <v>28</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -4740,7 +4928,7 @@
         <v>20</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4748,7 +4936,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4756,7 +4944,7 @@
         <v>21</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4764,7 +4952,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4803,7 +4991,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" ht="30" customHeight="1">
       <c r="B58" s="4"/>
       <c r="C58" s="6" t="s">
         <v>78</v>
@@ -4814,7 +5002,7 @@
         <v>24</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -4822,12 +5010,12 @@
         <v>23</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>58</v>
@@ -4836,28 +5024,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30" customHeight="1">
+    <row r="62" spans="1:3" ht="45">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="B63" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C63" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" customHeight="1">
+      <c r="B64" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" s="4" t="s">
-        <v>230</v>
-      </c>
       <c r="C64" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -4865,20 +5053,20 @@
         <v>26</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>58</v>
@@ -4887,7 +5075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30" customHeight="1">
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>50</v>
       </c>
@@ -4900,7 +5088,7 @@
         <v>4</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>79</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -4925,6 +5113,41 @@
       </c>
       <c r="C72" s="5" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30">
+      <c r="A74" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4936,7 +5159,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="10">
+  <tableParts count="11">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -4947,6 +5170,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4986,25 +5210,25 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5086,16 +5310,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5166,7 +5390,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -5280,7 +5504,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>19</v>
@@ -5292,13 +5516,13 @@
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>20</v>
@@ -5321,770 +5545,770 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -6149,16 +6373,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -6187,7 +6411,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6303,6 +6527,77 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="136.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" ht="15">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:H12"/>
@@ -6326,7 +6621,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -6335,7 +6630,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
@@ -6344,7 +6639,7 @@
         <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -6384,7 +6679,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>29</v>
@@ -6409,7 +6704,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8">

</xml_diff>

<commit_message>
update msg and improve documentation on submission spreadsheet
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="736"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="10" r:id="rId1"/>
@@ -194,15 +194,6 @@
     <t>Chromosome where the Target is located</t>
   </si>
   <si>
-    <t>Start location of the Target in the assembly</t>
-  </si>
-  <si>
-    <t>End location of the Target in the assembly</t>
-  </si>
-  <si>
-    <t>Strand location of the Target in the assembly either "forward" or "reverse"</t>
-  </si>
-  <si>
     <t>Nucleotide sequence of the guide, e.g. GAGATTATGAAACACCAAAG</t>
   </si>
   <si>
@@ -216,26 +207,6 @@
   </si>
   <si>
     <t>How many offtargets that contain x number of mismatches</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Amplicon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> is the DNA sequence amplified in PCR by a primer pair. All sequences and sequence locations input here must be in the forward DNA strand (including guide, forward and reverse primers)</t>
-    </r>
   </si>
   <si>
     <t>knock-in or knock-out</t>
@@ -759,33 +730,7 @@
     <t>Is this amplicon on-target or off-target? (TRUE/FALSE)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The name of one of the guide defined in the Guide tab, it must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Guide@guide_name</t>
-    </r>
-  </si>
-  <si>
     <t>Name of the guide</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The name of one of the target defined in the Target tab, it must match one of </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Target@target_name</t>
-    </r>
   </si>
   <si>
     <t>The name of the Target. This name must be unique within this project.</t>
@@ -868,6 +813,405 @@
     </r>
   </si>
   <si>
+    <t>unique ID for a layout plate, e.g. plate_01</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> The type of the sequencing library e.g. Fluidigm</t>
+    </r>
+  </si>
+  <si>
+    <t>The barcode identifier, e.g. FLD0193 which is part of the fastq file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> The sample name assigned at the time of submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> The Sequencing project ID the NGS library was assigned to, e.g. SLX-13775</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> The starting material used for library preparation, either of fixed cells, gDNA, non-fixed cells</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Name of the parental cell line used to derive a clone (if any) to gene-edit, e.g MCF7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Name of the parental cell line-derived clone. This is the source of cells used to gene-edit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Is there a control in this well position? (TRUE/FALSE) Default set to False</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Off-target score as provided by Deskgen (leave targets empty)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Plate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> collects information on the unique ID's and barcodes assigned to each plate over an experiment. A plate Layout (distribution of wells and associated information) for a plate is unique, and that Layout is associated to results from ICW, IncuCyte and NGS.</t>
+    </r>
+  </si>
+  <si>
+    <t>layout_geid</t>
+  </si>
+  <si>
+    <t>layout_id</t>
+  </si>
+  <si>
+    <t>plate_name</t>
+  </si>
+  <si>
+    <t>plate_description</t>
+  </si>
+  <si>
+    <t>The experimental plate name e.g. plate_01_incu, plate_01_ICW, plate_01_PCR, plate_01_NGS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Any description that can be informative about the plate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Unique barcode assigned to each individual plate, unique across all projects</t>
+    </r>
+  </si>
+  <si>
+    <t>NB. Orange tabs, tables and columns need to be filled, green ones are optionals.</t>
+  </si>
+  <si>
+    <t>is_true_or_false</t>
+  </si>
+  <si>
+    <t>GenEditID - Project Data and Layout Spreadsheet</t>
+  </si>
+  <si>
+    <t>Help to fill project's data and layout before uploading into the GenEditID Web App</t>
+  </si>
+  <si>
+    <t>knock-in</t>
+  </si>
+  <si>
+    <t>sequence_name</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>The name of the sequence</t>
+  </si>
+  <si>
+    <t>The sequence</t>
+  </si>
+  <si>
+    <t>amplicon_name</t>
+  </si>
+  <si>
+    <t>The name of the Amplicon. This name must be unique within this project.</t>
+  </si>
+  <si>
+    <t>TargetedSearch</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>TargetedSearch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> is a list of sequences that the reads are counted against. If looking for particular gene edits, the desired edited sequences should be put in here. If no sequence is provided, the amplicon as identified by the provided primer sequences will be considered for counting reads.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The name of one of the target defined in the Target tab, it must match one of </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>target_name@Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The name of one of the guide defined in the Guide tab, it must match </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>guide_name@Guide</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This ID must match </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>layout_id@Layout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This name must match </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>guide_name@Guide</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>This name must match</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> amplicon_name@Amplicon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <t>Start location of the Target in the assembly as on reference genome</t>
+  </si>
+  <si>
+    <t>End location of the Target in the assembly as on reference genome</t>
+  </si>
+  <si>
+    <t>Strand location of the Target in the assembly either "forward" or "reverse" as on reference genome</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Amplicon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> is the DNA sequence amplified in PCR by a primer pair. All sequences and sequence locations input here must be in the forward DNA strand as on reference genome (including guide, forward and reverse primers)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">The </t>
     </r>
@@ -884,316 +1228,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> describes the way samples are arranged in the plate wells, so ultimately any result can be traced back to a single clone. Each plate in the layout gets a unique ID, so clones are defined by a combination of plate geid and well_position.</t>
-    </r>
-  </si>
-  <si>
-    <t>unique ID for a layout plate, e.g. plate_01</t>
-  </si>
-  <si>
-    <t>Layout</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> The type of the sequencing library e.g. Fluidigm</t>
-    </r>
-  </si>
-  <si>
-    <t>The barcode identifier, e.g. FLD0193 which is part of the fastq file</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> The sample name assigned at the time of submission</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> The Sequencing project ID the NGS library was assigned to, e.g. SLX-13775</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> The starting material used for library preparation, either of fixed cells, gDNA, non-fixed cells</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Name of the parental cell line used to derive a clone (if any) to gene-edit, e.g MCF7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Name of the parental cell line-derived clone. This is the source of cells used to gene-edit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Is there a control in this well position? (TRUE/FALSE) Default set to False</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Off-target score as provided by Deskgen (leave targets empty)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Plate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> collects information on the unique ID's and barcodes assigned to each plate over an experiment. A plate Layout (distribution of wells and associated information) for a plate is unique, and that Layout is associated to results from ICW, IncuCyte and NGS.</t>
-    </r>
-  </si>
-  <si>
-    <t>layout_geid</t>
-  </si>
-  <si>
-    <t>layout_id</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This ID must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Layout@layout_id</t>
-    </r>
-  </si>
-  <si>
-    <t>plate_name</t>
-  </si>
-  <si>
-    <t>plate_description</t>
-  </si>
-  <si>
-    <t>The experimental plate name e.g. plate_01_incu, plate_01_ICW, plate_01_PCR, plate_01_NGS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Any description that can be informative about the plate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>[optional]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Unique barcode assigned to each individual plate, unique across all projects</t>
-    </r>
-  </si>
-  <si>
-    <t>NB. Orange tabs, tables and columns need to be filled, green ones are optionals.</t>
-  </si>
-  <si>
-    <t>is_true_or_false</t>
-  </si>
-  <si>
-    <t>GenEditID - Project Data and Layout Spreadsheet</t>
-  </si>
-  <si>
-    <t>Help to fill project's data and layout before uploading into the GenEditID Web App</t>
-  </si>
-  <si>
-    <t>knock-in</t>
-  </si>
-  <si>
-    <t>sequence_name</t>
-  </si>
-  <si>
-    <t>sequence</t>
-  </si>
-  <si>
-    <t>The name of the sequence</t>
-  </si>
-  <si>
-    <t>The sequence</t>
-  </si>
-  <si>
-    <t>amplicon_name</t>
-  </si>
-  <si>
-    <t>The name of the Amplicon. This name must be unique within this project.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This name must match </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Guide@guide_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>This name must match</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Amplicon@amplicon_name</t>
-    </r>
-  </si>
-  <si>
-    <t>TargetedSearch</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>TargetedSearch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> is a list of sequences that the reads are counted against. If looking for particular gene edits, the desired edited sequences should be put in here. If no sequence is provided, the amplicon as identified by the provided primer sequences will be considered for counting reads.</t>
+      <t xml:space="preserve"> describes the way samples are arranged in the plate wells, so ultimately any result can be traced back to a single clone. Each plate in the layout gets a unique ID, so clones are defined by a combination of plate layout_id and well_position.</t>
     </r>
   </si>
 </sst>
@@ -1320,7 +1355,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1364,6 +1399,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1558,7 +1595,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1660,6 +1697,7 @@
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1762,6 +1800,7 @@
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
@@ -4573,7 +4612,7 @@
   </sheetPr>
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -4587,31 +4626,31 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32">
       <c r="A1" s="18" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="19" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="20" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>52</v>
@@ -4622,7 +4661,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4630,28 +4669,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>53</v>
@@ -4659,43 +4698,43 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>52</v>
@@ -4707,7 +4746,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4715,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4723,7 +4762,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4731,47 +4770,47 @@
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>52</v>
@@ -4779,18 +4818,18 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>62</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4798,7 +4837,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4806,7 +4845,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4814,7 +4853,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -4822,7 +4861,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4830,15 +4869,15 @@
         <v>12</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4846,7 +4885,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4854,7 +4893,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4862,7 +4901,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="9" customFormat="1">
@@ -4871,7 +4910,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4879,7 +4918,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4887,7 +4926,7 @@
         <v>18</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
@@ -4896,7 +4935,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15">
@@ -4905,15 +4944,15 @@
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>52</v>
@@ -4921,18 +4960,18 @@
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -4940,7 +4979,7 @@
         <v>19</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -4948,23 +4987,23 @@
         <v>27</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -4972,15 +5011,15 @@
         <v>28</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4988,7 +5027,7 @@
         <v>20</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4996,7 +5035,7 @@
         <v>22</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -5004,7 +5043,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5012,49 +5051,49 @@
         <v>25</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" s="4"/>
       <c r="C53" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="4"/>
       <c r="C54" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="4"/>
       <c r="C55" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="4"/>
       <c r="C56" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="B57" s="4"/>
       <c r="C57" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30" customHeight="1">
       <c r="B58" s="4"/>
       <c r="C58" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="B59" s="4"/>
       <c r="C59" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -5062,7 +5101,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -5070,15 +5109,15 @@
         <v>23</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>52</v>
@@ -5089,23 +5128,23 @@
         <v>51</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30" customHeight="1">
       <c r="B64" s="4" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -5113,23 +5152,23 @@
         <v>26</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>52</v>
@@ -5140,7 +5179,7 @@
         <v>50</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -5148,7 +5187,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -5156,7 +5195,7 @@
         <v>5</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -5164,7 +5203,7 @@
         <v>6</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -5172,15 +5211,15 @@
         <v>7</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>52</v>
@@ -5188,34 +5227,34 @@
     </row>
     <row r="75" spans="1:3" ht="45">
       <c r="A75" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="B78" s="10" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -5255,7 +5294,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5278,25 +5317,25 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5378,16 +5417,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -5443,7 +5482,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>4</v>
@@ -5461,7 +5500,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>13</v>
@@ -5576,7 +5615,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>19</v>
@@ -5588,13 +5627,13 @@
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>20</v>
@@ -5617,770 +5656,770 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -6445,16 +6484,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6616,13 +6655,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15">
       <c r="A1" s="17" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15">
@@ -6705,7 +6744,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -6714,7 +6753,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
@@ -6723,7 +6762,7 @@
         <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -6763,7 +6802,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>29</v>
@@ -6788,7 +6827,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8">

</xml_diff>

<commit_message>
add support for multiple genomes at the loading steps, still work to be done for analysing the variants
</commit_message>
<xml_diff>
--- a/data/templates/GEPXXXXX.xlsx
+++ b/data/templates/GEPXXXXX.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="254">
   <si>
     <t>description</t>
   </si>
@@ -1248,12 +1248,24 @@
   <si>
     <t>refseq_orientation_match</t>
   </si>
+  <si>
+    <t>Mus musculus [GRCm39]</t>
+  </si>
+  <si>
+    <t>Rattus norvegicus [mRatBN7]</t>
+  </si>
+  <si>
+    <t>Danio rerio [GRCz11]</t>
+  </si>
+  <si>
+    <t>Drosophila melanogaster [BDGP6]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1351,16 +1363,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1392,6 +1415,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4F81BD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4F81BD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4F81BD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1644,7 +1682,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1675,6 +1713,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4797,7 +4837,7 @@
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -5569,7 +5609,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Menus!$A$2:$A$2</xm:f>
+            <xm:f>Menus!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B10</xm:sqref>
         </x14:dataValidation>
@@ -6927,13 +6967,11 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="3"/>
     <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -6968,7 +7006,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -6991,6 +7029,9 @@
       </c>
     </row>
     <row r="3" spans="1:8">
+      <c r="A3" s="23" t="s">
+        <v>250</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
@@ -7011,6 +7052,9 @@
       </c>
     </row>
     <row r="4" spans="1:8">
+      <c r="A4" s="22" t="s">
+        <v>251</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>35</v>
       </c>
@@ -7022,6 +7066,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" s="23" t="s">
+        <v>252</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
@@ -7030,6 +7077,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" s="22" t="s">
+        <v>253</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>41</v>
       </c>

</xml_diff>